<commit_message>
Analiza wyników - t-Student + autorski opis
</commit_message>
<xml_diff>
--- a/wyniki.xlsx
+++ b/wyniki.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="85">
   <si>
     <t>Bartek_2</t>
   </si>
@@ -1260,6 +1260,9 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>http://www.socscistatistics.com/tests/studentttest/Default2.aspx</t>
   </si>
 </sst>
 </file>
@@ -5227,7 +5230,7 @@
   <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G13"/>
+      <selection activeCell="L1" sqref="L1:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6203,8 +6206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X13"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11972,7 +11975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
@@ -16275,10 +16278,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:X87"/>
+  <dimension ref="A2:X90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G87" sqref="G87"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22363,6 +22366,11 @@
         <v>-0.21366815983794593</v>
       </c>
     </row>
+    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Analiza wyników - Autorska metoda translacji wyników w skali porównawczej na skalę pięciostopniową
</commit_message>
<xml_diff>
--- a/wyniki.xlsx
+++ b/wyniki.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
-    <sheet name="WynikiScenariusza1" sheetId="3" r:id="rId2"/>
-    <sheet name="WynikiScenariusza2" sheetId="4" r:id="rId3"/>
-    <sheet name="Wykresy" sheetId="7" r:id="rId4"/>
-    <sheet name="ANOVA" sheetId="5" r:id="rId5"/>
-    <sheet name="t-Student" sheetId="6" r:id="rId6"/>
-    <sheet name="t-Student2" sheetId="9" r:id="rId7"/>
+    <sheet name="WynikiScenariusza3" sheetId="10" r:id="rId2"/>
+    <sheet name="WynikiScenariusza1" sheetId="3" r:id="rId3"/>
+    <sheet name="WynikiScenariusza2" sheetId="4" r:id="rId4"/>
+    <sheet name="Wykresy" sheetId="7" r:id="rId5"/>
+    <sheet name="ANOVA" sheetId="5" r:id="rId6"/>
+    <sheet name="t-Student" sheetId="6" r:id="rId7"/>
+    <sheet name="t-Student2" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="101">
   <si>
     <t>Bartek_2</t>
   </si>
@@ -1264,6 +1265,54 @@
   <si>
     <t>http://www.socscistatistics.com/tests/studentttest/Default2.aspx</t>
   </si>
+  <si>
+    <t>PUPPIES.mp4_7000k.raw</t>
+  </si>
+  <si>
+    <t>PUPPIES.mp4_1500k.raw</t>
+  </si>
+  <si>
+    <t>PUPPIES.mp4_9000k.raw</t>
+  </si>
+  <si>
+    <t>PUPPIES.mp4_4000k.raw</t>
+  </si>
+  <si>
+    <t>Chimei.mp4_1500k.raw</t>
+  </si>
+  <si>
+    <t>PUPPIES.mp4_3000k.raw</t>
+  </si>
+  <si>
+    <t>PUPPIES.mp4_2000k.raw</t>
+  </si>
+  <si>
+    <t>Chimei.mp4_2000k.raw</t>
+  </si>
+  <si>
+    <t>Puppies_9000k</t>
+  </si>
+  <si>
+    <t>Puppies_7000k</t>
+  </si>
+  <si>
+    <t>Puppies_4000k</t>
+  </si>
+  <si>
+    <t>Puppies_3000k</t>
+  </si>
+  <si>
+    <t>Puppies_1500k</t>
+  </si>
+  <si>
+    <t>Chimei_1500k</t>
+  </si>
+  <si>
+    <t>Chimei_2000k</t>
+  </si>
+  <si>
+    <t>Puppies_2000k</t>
+  </si>
 </sst>
 </file>
 
@@ -1332,7 +1381,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1375,8 +1424,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1384,12 +1439,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1401,6 +1508,29 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -1640,11 +1770,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="171582432"/>
-        <c:axId val="171582992"/>
+        <c:axId val="173219616"/>
+        <c:axId val="173220176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="171582432"/>
+        <c:axId val="173219616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1686,7 +1816,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="171582992"/>
+        <c:crossAx val="173220176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1694,7 +1824,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="171582992"/>
+        <c:axId val="173220176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1745,7 +1875,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="171582432"/>
+        <c:crossAx val="173219616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2637,8 +2767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R21" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="P39" sqref="P39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5227,10 +5357,860 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X13"/>
+  <dimension ref="A1:X31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1" s="9">
+        <v>-1</v>
+      </c>
+      <c r="E1" s="9">
+        <v>-2</v>
+      </c>
+      <c r="F1" s="9">
+        <v>0</v>
+      </c>
+      <c r="G1" s="9">
+        <v>-1</v>
+      </c>
+      <c r="H1" s="9">
+        <v>2</v>
+      </c>
+      <c r="I1" s="9">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="9">
+        <v>-2</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0</v>
+      </c>
+      <c r="G2" s="9">
+        <v>0</v>
+      </c>
+      <c r="H2" s="9">
+        <v>0</v>
+      </c>
+      <c r="I2" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="9">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9">
+        <v>-1</v>
+      </c>
+      <c r="E3" s="9">
+        <v>-2</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0</v>
+      </c>
+      <c r="I3" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="9">
+        <v>-3</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="9">
+        <v>-3</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
+        <v>-1</v>
+      </c>
+      <c r="H5" s="9">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9">
+        <v>-1</v>
+      </c>
+      <c r="E6" s="9">
+        <v>-3</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9">
+        <v>1</v>
+      </c>
+      <c r="I6" s="9">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9">
+        <v>-1</v>
+      </c>
+      <c r="E7" s="9">
+        <v>-3</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <v>-1</v>
+      </c>
+      <c r="H7" s="9">
+        <v>0</v>
+      </c>
+      <c r="I7" s="9">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="9">
+        <v>-1</v>
+      </c>
+      <c r="D8" s="9">
+        <v>-1</v>
+      </c>
+      <c r="E8" s="9">
+        <v>-2</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9">
+        <v>-3</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0</v>
+      </c>
+      <c r="I8" s="9">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="9">
+        <v>-1</v>
+      </c>
+      <c r="E9" s="9">
+        <v>-2</v>
+      </c>
+      <c r="F9" s="9">
+        <v>-3</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <v>-3</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0</v>
+      </c>
+      <c r="H10" s="9">
+        <v>0</v>
+      </c>
+      <c r="I10" s="9">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0</v>
+      </c>
+      <c r="D11" s="9">
+        <v>-2</v>
+      </c>
+      <c r="E11" s="9">
+        <v>-2</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0</v>
+      </c>
+      <c r="G11" s="9">
+        <v>-1</v>
+      </c>
+      <c r="H11" s="9">
+        <v>1</v>
+      </c>
+      <c r="I11" s="9">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="9">
+        <v>-1</v>
+      </c>
+      <c r="D12" s="9">
+        <v>-2</v>
+      </c>
+      <c r="E12" s="9">
+        <v>-3</v>
+      </c>
+      <c r="F12" s="9">
+        <v>-2</v>
+      </c>
+      <c r="G12" s="9">
+        <v>-2</v>
+      </c>
+      <c r="H12" s="9">
+        <v>-1</v>
+      </c>
+      <c r="I12" s="9">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="9">
+        <v>-1</v>
+      </c>
+      <c r="D13" s="9">
+        <v>-2</v>
+      </c>
+      <c r="E13" s="9">
+        <v>-2</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>1</v>
+      </c>
+      <c r="I13" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+    </row>
+    <row r="23" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" t="s">
+        <v>3</v>
+      </c>
+      <c r="M23" t="s">
+        <v>6</v>
+      </c>
+      <c r="N23" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P23" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>17</v>
+      </c>
+      <c r="R23" t="s">
+        <v>20</v>
+      </c>
+      <c r="S23" t="s">
+        <v>23</v>
+      </c>
+      <c r="T23" t="s">
+        <v>26</v>
+      </c>
+      <c r="U23" t="s">
+        <v>29</v>
+      </c>
+      <c r="V23" t="s">
+        <v>32</v>
+      </c>
+      <c r="W23" t="s">
+        <v>35</v>
+      </c>
+      <c r="X23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="L24" s="13">
+        <v>5</v>
+      </c>
+      <c r="M24" s="13">
+        <v>5</v>
+      </c>
+      <c r="N24" s="17"/>
+      <c r="O24" s="13">
+        <v>5</v>
+      </c>
+      <c r="P24" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q24" s="13">
+        <v>5</v>
+      </c>
+      <c r="R24" s="13">
+        <v>4</v>
+      </c>
+      <c r="S24" s="13">
+        <v>5</v>
+      </c>
+      <c r="T24" s="13">
+        <v>5</v>
+      </c>
+      <c r="U24" s="13">
+        <v>5</v>
+      </c>
+      <c r="V24" s="13">
+        <v>5</v>
+      </c>
+      <c r="W24" s="13">
+        <v>5</v>
+      </c>
+      <c r="X24" s="13"/>
+    </row>
+    <row r="25" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="L25" s="15">
+        <v>5</v>
+      </c>
+      <c r="M25" s="15">
+        <v>5</v>
+      </c>
+      <c r="N25" s="18"/>
+      <c r="O25" s="15">
+        <v>5</v>
+      </c>
+      <c r="P25" s="15">
+        <v>5</v>
+      </c>
+      <c r="Q25" s="15">
+        <v>5</v>
+      </c>
+      <c r="R25" s="15">
+        <v>5</v>
+      </c>
+      <c r="S25" s="15">
+        <v>4</v>
+      </c>
+      <c r="T25" s="15">
+        <v>5</v>
+      </c>
+      <c r="U25" s="15">
+        <v>5</v>
+      </c>
+      <c r="V25" s="15">
+        <v>5</v>
+      </c>
+      <c r="W25" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="X25" s="15"/>
+    </row>
+    <row r="26" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="L26" s="15">
+        <v>4</v>
+      </c>
+      <c r="M26" s="15">
+        <v>3</v>
+      </c>
+      <c r="N26" s="18"/>
+      <c r="O26" s="15">
+        <v>4</v>
+      </c>
+      <c r="P26" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="Q26" s="15">
+        <v>4</v>
+      </c>
+      <c r="R26" s="15">
+        <v>4</v>
+      </c>
+      <c r="S26" s="15">
+        <v>4</v>
+      </c>
+      <c r="T26" s="15">
+        <v>4</v>
+      </c>
+      <c r="U26" s="15">
+        <v>5</v>
+      </c>
+      <c r="V26" s="15">
+        <v>4</v>
+      </c>
+      <c r="W26" s="15">
+        <v>4</v>
+      </c>
+      <c r="X26" s="15"/>
+    </row>
+    <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="L27" s="15">
+        <v>2</v>
+      </c>
+      <c r="M27" s="15">
+        <v>2</v>
+      </c>
+      <c r="N27" s="18"/>
+      <c r="O27" s="15">
+        <v>2</v>
+      </c>
+      <c r="P27" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="Q27" s="15">
+        <v>3</v>
+      </c>
+      <c r="R27" s="15">
+        <v>2</v>
+      </c>
+      <c r="S27" s="15">
+        <v>3</v>
+      </c>
+      <c r="T27" s="15">
+        <v>1</v>
+      </c>
+      <c r="U27" s="15">
+        <v>3</v>
+      </c>
+      <c r="V27" s="15">
+        <v>3</v>
+      </c>
+      <c r="W27" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="X27" s="15"/>
+    </row>
+    <row r="28" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="L28" s="15">
+        <v>3</v>
+      </c>
+      <c r="M28" s="15">
+        <v>2</v>
+      </c>
+      <c r="N28" s="18"/>
+      <c r="O28" s="15">
+        <v>2</v>
+      </c>
+      <c r="P28" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="Q28" s="15">
+        <v>3</v>
+      </c>
+      <c r="R28" s="15">
+        <v>3</v>
+      </c>
+      <c r="S28" s="15">
+        <v>3</v>
+      </c>
+      <c r="T28" s="19">
+        <v>4</v>
+      </c>
+      <c r="U28" s="15">
+        <v>3</v>
+      </c>
+      <c r="V28" s="15">
+        <v>4</v>
+      </c>
+      <c r="W28" s="15">
+        <v>4</v>
+      </c>
+      <c r="X28" s="15"/>
+    </row>
+    <row r="29" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="L29" s="15">
+        <v>3</v>
+      </c>
+      <c r="M29" s="15">
+        <v>2</v>
+      </c>
+      <c r="N29" s="18"/>
+      <c r="O29" s="15">
+        <v>2</v>
+      </c>
+      <c r="P29" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="Q29" s="15">
+        <v>3</v>
+      </c>
+      <c r="R29" s="15">
+        <v>3</v>
+      </c>
+      <c r="S29" s="15">
+        <v>3</v>
+      </c>
+      <c r="T29" s="15">
+        <v>1</v>
+      </c>
+      <c r="U29" s="15">
+        <v>3</v>
+      </c>
+      <c r="V29" s="15">
+        <v>4</v>
+      </c>
+      <c r="W29" s="15">
+        <v>2</v>
+      </c>
+      <c r="X29" s="15"/>
+    </row>
+    <row r="30" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="L30" s="15">
+        <v>2</v>
+      </c>
+      <c r="M30" s="15">
+        <v>2</v>
+      </c>
+      <c r="N30" s="18"/>
+      <c r="O30" s="15">
+        <v>2</v>
+      </c>
+      <c r="P30" s="15">
+        <v>3</v>
+      </c>
+      <c r="Q30" s="15">
+        <v>3</v>
+      </c>
+      <c r="R30" s="15">
+        <v>2</v>
+      </c>
+      <c r="S30" s="15">
+        <v>1</v>
+      </c>
+      <c r="T30" s="15">
+        <v>1</v>
+      </c>
+      <c r="U30" s="15">
+        <v>3</v>
+      </c>
+      <c r="V30" s="15">
+        <v>3</v>
+      </c>
+      <c r="W30" s="15">
+        <v>1</v>
+      </c>
+      <c r="X30" s="15"/>
+    </row>
+    <row r="31" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K31" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="L31" s="15">
+        <v>1</v>
+      </c>
+      <c r="M31" s="15">
+        <v>1</v>
+      </c>
+      <c r="N31" s="18"/>
+      <c r="O31" s="15">
+        <v>1</v>
+      </c>
+      <c r="P31" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="15">
+        <v>1</v>
+      </c>
+      <c r="R31" s="15">
+        <v>1</v>
+      </c>
+      <c r="S31" s="15">
+        <v>1</v>
+      </c>
+      <c r="T31" s="15">
+        <v>1</v>
+      </c>
+      <c r="U31" s="15">
+        <v>1</v>
+      </c>
+      <c r="V31" s="15">
+        <v>1</v>
+      </c>
+      <c r="W31" s="15">
+        <v>1</v>
+      </c>
+      <c r="X31" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L13"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6197,12 +7177,22 @@
         <v>2</v>
       </c>
     </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f>AVERAGE(C1:C13)</f>
+        <v>1.2307692307692308</v>
+      </c>
+      <c r="H15">
+        <f>AVERAGE(H1:H13)</f>
+        <v>1.6153846153846154</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X13"/>
   <sheetViews>
@@ -7182,7 +8172,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X8"/>
   <sheetViews>
@@ -7799,7 +8789,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z68"/>
   <sheetViews>
@@ -11971,11 +12961,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
@@ -16276,12 +17266,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X90"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87:X87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20168,1223 +21158,1223 @@
     </row>
     <row r="53" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B53">
-        <f>POWER(B24,2)</f>
+        <f t="shared" ref="B53:B65" si="14">POWER(B24,2)</f>
         <v>0.59171597633136086</v>
       </c>
       <c r="C53">
-        <f t="shared" ref="C53:X53" si="14">POWER(C24,2)</f>
+        <f t="shared" ref="C53:X53" si="15">POWER(C24,2)</f>
         <v>5.9171597633136015E-3</v>
       </c>
       <c r="D53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="E53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.37869822485207105</v>
       </c>
       <c r="F53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="G53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.5147928994082842</v>
       </c>
       <c r="H53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.28994082840236696</v>
       </c>
       <c r="I53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.85207100591716023</v>
       </c>
       <c r="J53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="K53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.21301775147929006</v>
       </c>
       <c r="L53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.3668639053254406E-2</v>
       </c>
       <c r="M53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.9171597633135677E-3</v>
       </c>
       <c r="N53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.28994082840236673</v>
       </c>
       <c r="O53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="P53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.85207100591716023</v>
       </c>
       <c r="Q53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.71597633136094618</v>
       </c>
       <c r="R53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.59171597633136086</v>
       </c>
       <c r="S53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.3668639053254406E-2</v>
       </c>
       <c r="T53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.21301775147928986</v>
       </c>
       <c r="U53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.47928994082840265</v>
       </c>
       <c r="V53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="W53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.21301775147929006</v>
       </c>
       <c r="X53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.28994082840236673</v>
       </c>
     </row>
     <row r="54" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B54">
-        <f>POWER(B25,2)</f>
+        <f t="shared" si="14"/>
         <v>0.59171597633136086</v>
       </c>
       <c r="C54">
-        <f t="shared" ref="C54:X54" si="15">POWER(C25,2)</f>
+        <f t="shared" ref="C54:X54" si="16">POWER(C25,2)</f>
         <v>5.9171597633136015E-3</v>
       </c>
       <c r="D54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="E54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.37869822485207105</v>
       </c>
       <c r="F54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="G54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.5147928994082842</v>
       </c>
       <c r="H54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.28994082840236696</v>
       </c>
       <c r="I54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.85207100591716023</v>
       </c>
       <c r="J54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="K54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.1360946745562135</v>
       </c>
       <c r="L54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.3313609467455618</v>
       </c>
       <c r="M54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.85207100591716023</v>
       </c>
       <c r="N54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.28994082840236673</v>
       </c>
       <c r="O54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="P54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5.9171597633135677E-3</v>
       </c>
       <c r="Q54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.71597633136094618</v>
       </c>
       <c r="R54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.59171597633136086</v>
       </c>
       <c r="S54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.71597633136094696</v>
       </c>
       <c r="T54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.21301775147928986</v>
       </c>
       <c r="U54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.47928994082840265</v>
       </c>
       <c r="V54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.7100591715976325</v>
       </c>
       <c r="W54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.21301775147929006</v>
       </c>
       <c r="X54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.3668639053254434</v>
       </c>
     </row>
     <row r="55" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B55">
-        <f>POWER(B26,2)</f>
+        <f t="shared" si="14"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="C55">
-        <f t="shared" ref="C55:X55" si="16">POWER(C26,2)</f>
+        <f t="shared" ref="C55:X55" si="17">POWER(C26,2)</f>
         <v>5.9171597633136015E-3</v>
       </c>
       <c r="D55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="E55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.14792899408284022</v>
       </c>
       <c r="F55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="G55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="H55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.21301775147928986</v>
       </c>
       <c r="I55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5.9171597633135677E-3</v>
       </c>
       <c r="J55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="K55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.28994082840236673</v>
       </c>
       <c r="L55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2.3668639053254406E-2</v>
       </c>
       <c r="M55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5.9171597633135677E-3</v>
       </c>
       <c r="N55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.28994082840236673</v>
       </c>
       <c r="O55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.59171597633136086</v>
       </c>
       <c r="P55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.1597633136094669</v>
       </c>
       <c r="Q55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.71597633136094618</v>
       </c>
       <c r="R55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.59171597633136086</v>
       </c>
       <c r="S55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2.3668639053254406E-2</v>
       </c>
       <c r="T55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.28994082840236696</v>
       </c>
       <c r="U55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="V55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="W55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.28994082840236673</v>
       </c>
       <c r="X55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.28994082840236673</v>
       </c>
     </row>
     <row r="56" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B56">
-        <f>POWER(B27,2)</f>
+        <f t="shared" si="14"/>
         <v>0.59171597633136086</v>
       </c>
       <c r="C56">
-        <f t="shared" ref="C56:X56" si="17">POWER(C27,2)</f>
+        <f t="shared" ref="C56:X56" si="18">POWER(C27,2)</f>
         <v>5.9171597633136015E-3</v>
       </c>
       <c r="D56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="E56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.37869822485207105</v>
       </c>
       <c r="F56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="G56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="H56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.21301775147928986</v>
       </c>
       <c r="I56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.85207100591716023</v>
       </c>
       <c r="J56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="K56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.21301775147929006</v>
       </c>
       <c r="L56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.3668639053254406E-2</v>
       </c>
       <c r="M56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>5.9171597633135677E-3</v>
       </c>
       <c r="N56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.28994082840236673</v>
       </c>
       <c r="O56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="P56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.85207100591716023</v>
       </c>
       <c r="Q56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.3668639053254541E-2</v>
       </c>
       <c r="R56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="S56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.71597633136094696</v>
       </c>
       <c r="T56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.21301775147928986</v>
       </c>
       <c r="U56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="V56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="W56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.21301775147929006</v>
       </c>
       <c r="X56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.28994082840236673</v>
       </c>
     </row>
     <row r="57" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B57">
-        <f>POWER(B28,2)</f>
+        <f t="shared" si="14"/>
         <v>0.59171597633136086</v>
       </c>
       <c r="C57">
-        <f t="shared" ref="C57:X57" si="18">POWER(C28,2)</f>
+        <f t="shared" ref="C57:X57" si="19">POWER(C28,2)</f>
         <v>0.8520710059171599</v>
       </c>
       <c r="D57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2.8639053254437878</v>
       </c>
       <c r="E57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.37869822485207105</v>
       </c>
       <c r="F57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="G57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="H57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.28994082840236696</v>
       </c>
       <c r="I57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.1597633136094669</v>
       </c>
       <c r="J57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="K57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.28994082840236673</v>
       </c>
       <c r="L57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2.3668639053254406E-2</v>
       </c>
       <c r="M57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.85207100591716023</v>
       </c>
       <c r="N57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2.1360946745562135</v>
       </c>
       <c r="O57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="P57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5.9171597633135677E-3</v>
       </c>
       <c r="Q57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.3313609467455629</v>
       </c>
       <c r="R57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="S57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2.3668639053254406E-2</v>
       </c>
       <c r="T57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.28994082840236696</v>
       </c>
       <c r="U57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.47928994082840265</v>
       </c>
       <c r="V57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="W57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.21301775147929006</v>
       </c>
       <c r="X57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.28994082840236673</v>
       </c>
     </row>
     <row r="58" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B58">
-        <f>POWER(B29,2)</f>
+        <f t="shared" si="14"/>
         <v>1.5147928994082842</v>
       </c>
       <c r="C58">
-        <f t="shared" ref="C58:X58" si="19">POWER(C29,2)</f>
+        <f t="shared" ref="C58:X58" si="20">POWER(C29,2)</f>
         <v>5.9171597633136015E-3</v>
       </c>
       <c r="D58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="E58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.14792899408284022</v>
       </c>
       <c r="F58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="G58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="H58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.21301775147928986</v>
       </c>
       <c r="I58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>5.9171597633135677E-3</v>
       </c>
       <c r="J58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="K58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.21301775147929006</v>
       </c>
       <c r="L58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.3668639053254406E-2</v>
       </c>
       <c r="M58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>5.9171597633135677E-3</v>
       </c>
       <c r="N58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.21301775147929006</v>
       </c>
       <c r="O58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="P58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.85207100591716023</v>
       </c>
       <c r="Q58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.3668639053254541E-2</v>
       </c>
       <c r="R58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.59171597633136086</v>
       </c>
       <c r="S58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.3668639053254406E-2</v>
       </c>
       <c r="T58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.28994082840236696</v>
       </c>
       <c r="U58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="V58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="W58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.21301775147929006</v>
       </c>
       <c r="X58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.21301775147929006</v>
       </c>
     </row>
     <row r="59" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B59">
-        <f>POWER(B30,2)</f>
+        <f t="shared" si="14"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="C59">
-        <f t="shared" ref="C59:X59" si="20">POWER(C30,2)</f>
+        <f t="shared" ref="C59:X59" si="21">POWER(C30,2)</f>
         <v>5.9171597633136015E-3</v>
       </c>
       <c r="D59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="E59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.37869822485207105</v>
       </c>
       <c r="F59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="G59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="H59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.28994082840236696</v>
       </c>
       <c r="I59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.85207100591716023</v>
       </c>
       <c r="J59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="K59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.28994082840236673</v>
       </c>
       <c r="L59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.3313609467455618</v>
       </c>
       <c r="M59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.85207100591716023</v>
       </c>
       <c r="N59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.21301775147929006</v>
       </c>
       <c r="O59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="P59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>5.9171597633135677E-3</v>
       </c>
       <c r="Q59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2.3668639053254541E-2</v>
       </c>
       <c r="R59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.5147928994082842</v>
       </c>
       <c r="S59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.71597633136094696</v>
       </c>
       <c r="T59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.21301775147928986</v>
       </c>
       <c r="U59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.47928994082840265</v>
       </c>
       <c r="V59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="W59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.21301775147929006</v>
       </c>
       <c r="X59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.28994082840236673</v>
       </c>
     </row>
     <row r="60" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B60">
-        <f>POWER(B31,2)</f>
+        <f t="shared" si="14"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="C60">
-        <f t="shared" ref="C60:X60" si="21">POWER(C31,2)</f>
+        <f t="shared" ref="C60:X60" si="22">POWER(C31,2)</f>
         <v>5.9171597633136015E-3</v>
       </c>
       <c r="D60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="E60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.14792899408284022</v>
       </c>
       <c r="F60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>4</v>
       </c>
       <c r="G60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>7.6686390532544371</v>
       </c>
       <c r="H60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.21301775147928986</v>
       </c>
       <c r="I60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>4.3136094674556205</v>
       </c>
       <c r="J60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="K60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.28994082840236673</v>
       </c>
       <c r="L60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.71597633136094696</v>
       </c>
       <c r="M60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1.1597633136094669</v>
       </c>
       <c r="N60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.21301775147929006</v>
       </c>
       <c r="O60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="P60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1.1597633136094669</v>
       </c>
       <c r="Q60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>4.6390532544378713</v>
       </c>
       <c r="R60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="S60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>2.3668639053254406E-2</v>
       </c>
       <c r="T60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.21301775147928986</v>
       </c>
       <c r="U60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.47928994082840265</v>
       </c>
       <c r="V60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.47928994082840265</v>
       </c>
       <c r="W60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.28994082840236673</v>
       </c>
       <c r="X60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>2.1360946745562135</v>
       </c>
     </row>
     <row r="61" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B61">
-        <f>POWER(B32,2)</f>
+        <f t="shared" si="14"/>
         <v>1.5147928994082842</v>
       </c>
       <c r="C61">
-        <f t="shared" ref="C61:X61" si="22">POWER(C32,2)</f>
+        <f t="shared" ref="C61:X61" si="23">POWER(C32,2)</f>
         <v>5.9171597633136015E-3</v>
       </c>
       <c r="D61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="E61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.14792899408284022</v>
       </c>
       <c r="F61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="G61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.59171597633136086</v>
       </c>
       <c r="H61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.21301775147928986</v>
       </c>
       <c r="I61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>5.9171597633135677E-3</v>
       </c>
       <c r="J61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="K61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.28994082840236673</v>
       </c>
       <c r="L61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.71597633136094696</v>
       </c>
       <c r="M61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1.1597633136094669</v>
       </c>
       <c r="N61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.21301775147929006</v>
       </c>
       <c r="O61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.59171597633136086</v>
       </c>
       <c r="P61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1.1597633136094669</v>
       </c>
       <c r="Q61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.71597633136094618</v>
       </c>
       <c r="R61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1.5147928994082842</v>
       </c>
       <c r="S61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1.3313609467455618</v>
       </c>
       <c r="T61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.28994082840236696</v>
       </c>
       <c r="U61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="V61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.47928994082840265</v>
       </c>
       <c r="W61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.28994082840236673</v>
       </c>
       <c r="X61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2.1360946745562135</v>
       </c>
     </row>
     <row r="62" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B62">
-        <f>POWER(B33,2)</f>
+        <f t="shared" si="14"/>
         <v>0.59171597633136086</v>
       </c>
       <c r="C62">
-        <f t="shared" ref="C62:X62" si="23">POWER(C33,2)</f>
+        <f t="shared" ref="C62:X62" si="24">POWER(C33,2)</f>
         <v>5.9171597633136015E-3</v>
       </c>
       <c r="D62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.47928994082840265</v>
       </c>
       <c r="E62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.14792899408284022</v>
       </c>
       <c r="F62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="G62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="H62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.28994082840236696</v>
       </c>
       <c r="I62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>5.9171597633135677E-3</v>
       </c>
       <c r="J62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="K62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.21301775147929006</v>
       </c>
       <c r="L62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>2.3668639053254406E-2</v>
       </c>
       <c r="M62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.85207100591716023</v>
       </c>
       <c r="N62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.28994082840236673</v>
       </c>
       <c r="O62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="P62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.85207100591716023</v>
       </c>
       <c r="Q62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.71597633136094618</v>
       </c>
       <c r="R62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.59171597633136086</v>
       </c>
       <c r="S62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>2.3668639053254406E-2</v>
       </c>
       <c r="T62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.21301775147928986</v>
       </c>
       <c r="U62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.47928994082840265</v>
       </c>
       <c r="V62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="W62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.21301775147929006</v>
       </c>
       <c r="X62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.28994082840236673</v>
       </c>
     </row>
     <row r="63" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B63">
-        <f>POWER(B34,2)</f>
+        <f t="shared" si="14"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="C63">
-        <f t="shared" ref="C63:X63" si="24">POWER(C34,2)</f>
+        <f t="shared" ref="C63:X63" si="25">POWER(C34,2)</f>
         <v>5.9171597633136015E-3</v>
       </c>
       <c r="D63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="E63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.14792899408284022</v>
       </c>
       <c r="F63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="G63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.59171597633136086</v>
       </c>
       <c r="H63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.28994082840236696</v>
       </c>
       <c r="I63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>5.9171597633135677E-3</v>
       </c>
       <c r="J63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.28994082840236673</v>
       </c>
       <c r="L63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.71597633136094696</v>
       </c>
       <c r="M63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>5.9171597633135677E-3</v>
       </c>
       <c r="N63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.21301775147929006</v>
       </c>
       <c r="O63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="P63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.85207100591716023</v>
       </c>
       <c r="Q63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.71597633136094618</v>
       </c>
       <c r="R63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.59171597633136086</v>
       </c>
       <c r="S63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>2.3668639053254406E-2</v>
       </c>
       <c r="T63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.21301775147928986</v>
       </c>
       <c r="U63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1.7100591715976325</v>
       </c>
       <c r="V63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.47928994082840265</v>
       </c>
       <c r="W63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.28994082840236673</v>
       </c>
       <c r="X63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.21301775147929006</v>
       </c>
     </row>
     <row r="64" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B64">
-        <f>POWER(B35,2)</f>
+        <f t="shared" si="14"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="C64">
-        <f t="shared" ref="C64:X64" si="25">POWER(C35,2)</f>
+        <f t="shared" ref="C64:X64" si="26">POWER(C35,2)</f>
         <v>5.9171597633136015E-3</v>
       </c>
       <c r="D64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="E64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.14792899408284022</v>
       </c>
       <c r="F64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="G64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1.5147928994082842</v>
       </c>
       <c r="H64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.21301775147928986</v>
       </c>
       <c r="I64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>5.9171597633135677E-3</v>
       </c>
       <c r="J64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="K64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.21301775147929006</v>
       </c>
       <c r="L64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2.3668639053254406E-2</v>
       </c>
       <c r="M64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>5.9171597633135677E-3</v>
       </c>
       <c r="N64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.28994082840236673</v>
       </c>
       <c r="O64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="P64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>5.9171597633135677E-3</v>
       </c>
       <c r="Q64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2.3668639053254541E-2</v>
       </c>
       <c r="R64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="S64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2.3668639053254406E-2</v>
       </c>
       <c r="T64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.28994082840236696</v>
       </c>
       <c r="U64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>9.4674556213017624E-2</v>
       </c>
       <c r="V64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.47928994082840265</v>
       </c>
       <c r="W64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.21301775147929006</v>
       </c>
       <c r="X64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.21301775147929006</v>
       </c>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B65">
-        <f>POWER(B36,2)</f>
+        <f t="shared" si="14"/>
         <v>5.3254437869822514E-2</v>
       </c>
       <c r="C65">
-        <f t="shared" ref="C65:X65" si="26">POWER(C36,2)</f>
+        <f t="shared" ref="C65:X65" si="27">POWER(C36,2)</f>
         <v>5.9171597633136015E-3</v>
       </c>
       <c r="D65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.47928994082840265</v>
       </c>
       <c r="E65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.14792899408284022</v>
       </c>
       <c r="F65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="G65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.59171597633136086</v>
       </c>
       <c r="H65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.21301775147928986</v>
       </c>
       <c r="I65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>5.9171597633135677E-3</v>
       </c>
       <c r="J65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="K65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.28994082840236673</v>
       </c>
       <c r="L65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.71597633136094696</v>
       </c>
       <c r="M65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1.1597633136094669</v>
       </c>
       <c r="N65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.28994082840236673</v>
       </c>
       <c r="O65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.59171597633136086</v>
       </c>
       <c r="P65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1.1597633136094669</v>
       </c>
       <c r="Q65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1.3313609467455629</v>
       </c>
       <c r="R65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1.5147928994082842</v>
       </c>
       <c r="S65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>2.3668639053254406E-2</v>
       </c>
       <c r="T65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.28994082840236696</v>
       </c>
       <c r="U65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1.7100591715976325</v>
       </c>
       <c r="V65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.47928994082840265</v>
       </c>
       <c r="W65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>2.3668639053254434</v>
       </c>
       <c r="X65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.21301775147929006</v>
       </c>
     </row>
@@ -21397,87 +22387,87 @@
         <v>5.2307692307692317</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:W67" si="27">SUM(C39:C51)</f>
+        <f t="shared" ref="C67:W67" si="28">SUM(C39:C51)</f>
         <v>14.236686390532549</v>
       </c>
       <c r="D67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>1.9585798816568045</v>
       </c>
       <c r="E67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>9.0650887573964471</v>
       </c>
       <c r="F67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>5.1420118343195256</v>
       </c>
       <c r="G67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>7.1420118343195282</v>
       </c>
       <c r="H67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>10.988165680473372</v>
       </c>
       <c r="I67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>3.8816568047337281</v>
       </c>
       <c r="J67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>8.1301775147929014</v>
       </c>
       <c r="K67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>6.8106508875739644</v>
       </c>
       <c r="L67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>13.153846153846155</v>
       </c>
       <c r="M67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>7.1301775147929005</v>
       </c>
       <c r="N67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>5.1538461538461551</v>
       </c>
       <c r="O67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>12.207100591715975</v>
       </c>
       <c r="P67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>10.497041420118343</v>
       </c>
       <c r="Q67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>5.1420118343195256</v>
       </c>
       <c r="R67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>7.1301775147929014</v>
       </c>
       <c r="S67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>10.852071005917164</v>
       </c>
       <c r="T67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>15.698224852071011</v>
       </c>
       <c r="U67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>9.7278106508875748</v>
       </c>
       <c r="V67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>5.0650887573964507</v>
       </c>
       <c r="W67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>9.0000000000000018</v>
       </c>
       <c r="X67">
@@ -21494,87 +22484,87 @@
         <v>6.3076923076923075</v>
       </c>
       <c r="C68">
-        <f t="shared" ref="C68:W68" si="28">SUM(C53:C65)</f>
+        <f t="shared" ref="C68:W68" si="29">SUM(C53:C65)</f>
         <v>0.92307692307692346</v>
       </c>
       <c r="D68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>4.7692307692307692</v>
       </c>
       <c r="E68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>3.076923076923078</v>
       </c>
       <c r="F68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>10</v>
       </c>
       <c r="G68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>14.30769230769231</v>
       </c>
       <c r="H68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>3.2307692307692299</v>
       </c>
       <c r="I68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>8.9230769230769234</v>
       </c>
       <c r="J68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>12</v>
       </c>
       <c r="K68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>5.2307692307692317</v>
       </c>
       <c r="L68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>5.6923076923076925</v>
       </c>
       <c r="M68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>6.9230769230769242</v>
       </c>
       <c r="N68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>5.2307692307692317</v>
       </c>
       <c r="O68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>2.3076923076923079</v>
       </c>
       <c r="P68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>8.9230769230769234</v>
       </c>
       <c r="Q68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>11.69230769230769</v>
       </c>
       <c r="R68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>8.3076923076923084</v>
       </c>
       <c r="S68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>3.6923076923076934</v>
       </c>
       <c r="T68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>3.2307692307692304</v>
       </c>
       <c r="U68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>6.7692307692307692</v>
       </c>
       <c r="V68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>4.7692307692307701</v>
       </c>
       <c r="W68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>5.2307692307692317</v>
       </c>
       <c r="X68">
@@ -21591,87 +22581,87 @@
         <v>12</v>
       </c>
       <c r="C71">
-        <f t="shared" ref="C71:W72" si="29">13-1</f>
+        <f t="shared" ref="C71:W72" si="30">13-1</f>
         <v>12</v>
       </c>
       <c r="D71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="E71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="F71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="G71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="H71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="I71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="J71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="K71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="L71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="M71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="N71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="O71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="P71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="Q71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="R71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="S71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="T71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="U71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="V71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="W71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="X71">
@@ -21688,87 +22678,87 @@
         <v>12</v>
       </c>
       <c r="C72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="D72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="E72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="F72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="G72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="H72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="I72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="J72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="K72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="L72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="M72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="N72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="O72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="P72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="Q72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="R72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="S72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="T72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="U72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="V72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="W72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="X72">
@@ -21785,91 +22775,91 @@
         <v>0.43589743589743596</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:X75" si="30">C67/C71</f>
+        <f t="shared" ref="C75:X75" si="31">C67/C71</f>
         <v>1.1863905325443791</v>
       </c>
       <c r="D75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.16321499013806703</v>
       </c>
       <c r="E75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.75542406311637056</v>
       </c>
       <c r="F75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.4285009861932938</v>
       </c>
       <c r="G75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.59516765285996065</v>
       </c>
       <c r="H75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.91568047337278102</v>
       </c>
       <c r="I75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.32347140039447736</v>
       </c>
       <c r="J75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.67751479289940841</v>
       </c>
       <c r="K75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.56755424063116366</v>
       </c>
       <c r="L75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>1.0961538461538463</v>
       </c>
       <c r="M75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.59418145956607504</v>
       </c>
       <c r="N75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.42948717948717957</v>
       </c>
       <c r="O75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>1.0172583826429979</v>
       </c>
       <c r="P75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.87475345167652863</v>
       </c>
       <c r="Q75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.4285009861932938</v>
       </c>
       <c r="R75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.59418145956607515</v>
       </c>
       <c r="S75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.90433925049309705</v>
       </c>
       <c r="T75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>1.3081854043392509</v>
       </c>
       <c r="U75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.81065088757396453</v>
       </c>
       <c r="V75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.42209072978303758</v>
       </c>
       <c r="W75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.75000000000000011</v>
       </c>
       <c r="X75">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.91568047337278091</v>
       </c>
     </row>
@@ -21882,91 +22872,91 @@
         <v>0.52564102564102566</v>
       </c>
       <c r="C76">
-        <f t="shared" ref="C76:X76" si="31">C68/C72</f>
+        <f t="shared" ref="C76:X76" si="32">C68/C72</f>
         <v>7.6923076923076955E-2</v>
       </c>
       <c r="D76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.39743589743589741</v>
       </c>
       <c r="E76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.2564102564102565</v>
       </c>
       <c r="F76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="G76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1.1923076923076925</v>
       </c>
       <c r="H76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.26923076923076916</v>
       </c>
       <c r="I76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.74358974358974361</v>
       </c>
       <c r="J76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="K76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.43589743589743596</v>
       </c>
       <c r="L76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.47435897435897439</v>
       </c>
       <c r="M76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.57692307692307698</v>
       </c>
       <c r="N76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.43589743589743596</v>
       </c>
       <c r="O76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.19230769230769232</v>
       </c>
       <c r="P76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.74358974358974361</v>
       </c>
       <c r="Q76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.97435897435897412</v>
       </c>
       <c r="R76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.6923076923076924</v>
       </c>
       <c r="S76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.30769230769230776</v>
       </c>
       <c r="T76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.26923076923076922</v>
       </c>
       <c r="U76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.5641025641025641</v>
       </c>
       <c r="V76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.39743589743589752</v>
       </c>
       <c r="W76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.43589743589743596</v>
       </c>
       <c r="X76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.76923076923076927</v>
       </c>
     </row>
@@ -21981,91 +22971,91 @@
         <v>0.48076923076923084</v>
       </c>
       <c r="C79">
-        <f t="shared" ref="C79:X79" si="32" xml:space="preserve"> C71/(C71+C72)*C75 + C72/(C71+C72)*C76</f>
+        <f t="shared" ref="C79:X79" si="33" xml:space="preserve"> C71/(C71+C72)*C75 + C72/(C71+C72)*C76</f>
         <v>0.63165680473372798</v>
       </c>
       <c r="D79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.28032544378698221</v>
       </c>
       <c r="E79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.50591715976331353</v>
       </c>
       <c r="F79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.63091715976331364</v>
       </c>
       <c r="G79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89373767258382664</v>
       </c>
       <c r="H79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.59245562130177509</v>
       </c>
       <c r="I79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.53353057199211051</v>
       </c>
       <c r="J79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.83875739644970415</v>
       </c>
       <c r="K79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.50172583826429984</v>
       </c>
       <c r="L79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.78525641025641035</v>
       </c>
       <c r="M79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.58555226824457596</v>
       </c>
       <c r="N79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.43269230769230776</v>
       </c>
       <c r="O79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.60478303747534512</v>
       </c>
       <c r="P79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.80917159763313617</v>
       </c>
       <c r="Q79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.7014299802761339</v>
       </c>
       <c r="R79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.64324457593688378</v>
       </c>
       <c r="S79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.60601577909270243</v>
       </c>
       <c r="T79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.78870808678501003</v>
       </c>
       <c r="U79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.68737672583826437</v>
       </c>
       <c r="V79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.40976331360946755</v>
       </c>
       <c r="W79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.59294871794871806</v>
       </c>
       <c r="X79">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.84245562130177509</v>
       </c>
     </row>
@@ -22080,91 +23070,91 @@
         <v>3.6982248520710068E-2</v>
       </c>
       <c r="C82">
-        <f t="shared" ref="C82:X82" si="33">C79/13</f>
+        <f t="shared" ref="C82:X82" si="34">C79/13</f>
         <v>4.8588984979517538E-2</v>
       </c>
       <c r="D82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>2.1563495675921709E-2</v>
       </c>
       <c r="E82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>3.8916704597177963E-2</v>
       </c>
       <c r="F82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>4.8532089212562586E-2</v>
       </c>
       <c r="G82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>6.8749051737217431E-2</v>
       </c>
       <c r="H82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>4.5573509330905773E-2</v>
       </c>
       <c r="I82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>4.104081323016235E-2</v>
       </c>
       <c r="J82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>6.451979972690032E-2</v>
       </c>
       <c r="K82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>3.8594295251099989E-2</v>
       </c>
       <c r="L82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>6.0404339250493107E-2</v>
       </c>
       <c r="M82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>4.5042482172659687E-2</v>
       </c>
       <c r="N82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>3.3284023668639057E-2</v>
       </c>
       <c r="O82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>4.6521772113488083E-2</v>
       </c>
       <c r="P82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>6.2243969048702781E-2</v>
       </c>
       <c r="Q82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>5.3956152328933374E-2</v>
       </c>
       <c r="R82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>4.9480351995144903E-2</v>
       </c>
       <c r="S82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>4.6616598391746339E-2</v>
       </c>
       <c r="T82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>6.0669852829616157E-2</v>
       </c>
       <c r="U82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>5.2875132756789567E-2</v>
       </c>
       <c r="V82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>3.1520254893035962E-2</v>
       </c>
       <c r="W82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>4.5611439842209084E-2</v>
       </c>
       <c r="X82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>6.4804278561675005E-2</v>
       </c>
     </row>
@@ -22179,91 +23169,91 @@
         <v>3.6982248520710068E-2</v>
       </c>
       <c r="C84">
-        <f t="shared" ref="C84:X84" si="34">C79/13</f>
+        <f t="shared" ref="C84:X84" si="35">C79/13</f>
         <v>4.8588984979517538E-2</v>
       </c>
       <c r="D84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>2.1563495675921709E-2</v>
       </c>
       <c r="E84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>3.8916704597177963E-2</v>
       </c>
       <c r="F84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>4.8532089212562586E-2</v>
       </c>
       <c r="G84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>6.8749051737217431E-2</v>
       </c>
       <c r="H84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>4.5573509330905773E-2</v>
       </c>
       <c r="I84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>4.104081323016235E-2</v>
       </c>
       <c r="J84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>6.451979972690032E-2</v>
       </c>
       <c r="K84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>3.8594295251099989E-2</v>
       </c>
       <c r="L84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>6.0404339250493107E-2</v>
       </c>
       <c r="M84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>4.5042482172659687E-2</v>
       </c>
       <c r="N84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>3.3284023668639057E-2</v>
       </c>
       <c r="O84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>4.6521772113488083E-2</v>
       </c>
       <c r="P84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>6.2243969048702781E-2</v>
       </c>
       <c r="Q84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>5.3956152328933374E-2</v>
       </c>
       <c r="R84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>4.9480351995144903E-2</v>
       </c>
       <c r="S84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>4.6616598391746339E-2</v>
       </c>
       <c r="T84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>6.0669852829616157E-2</v>
       </c>
       <c r="U84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>5.2875132756789567E-2</v>
       </c>
       <c r="V84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>3.1520254893035962E-2</v>
       </c>
       <c r="W84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>4.5611439842209084E-2</v>
       </c>
       <c r="X84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>6.4804278561675005E-2</v>
       </c>
     </row>
@@ -22273,96 +23263,96 @@
       </c>
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B87">
+      <c r="B87" s="11">
         <f>(B2-B3)/SQRT(B82+B84)</f>
         <v>0.84852813742385713</v>
       </c>
-      <c r="C87">
-        <f t="shared" ref="C87:X87" si="35">(C2-C3)/SQRT(C82+C84)</f>
+      <c r="C87" s="11">
+        <f t="shared" ref="C87:X87" si="36">(C2-C3)/SQRT(C82+C84)</f>
         <v>0.49351769873992901</v>
       </c>
-      <c r="D87">
-        <f t="shared" si="35"/>
+      <c r="D87" s="11">
+        <f t="shared" si="36"/>
         <v>0.74081891505795661</v>
       </c>
-      <c r="E87">
-        <f t="shared" si="35"/>
+      <c r="E87" s="11">
+        <f t="shared" si="36"/>
         <v>0.82717019186851148</v>
       </c>
-      <c r="F87">
-        <f t="shared" si="35"/>
+      <c r="F87" s="11">
+        <f t="shared" si="36"/>
         <v>1.2345172438335541</v>
       </c>
-      <c r="G87">
-        <f t="shared" si="35"/>
+      <c r="G87" s="11">
+        <f t="shared" si="36"/>
         <v>-0.41489508437011219</v>
       </c>
-      <c r="H87">
-        <f t="shared" si="35"/>
+      <c r="H87" s="11">
+        <f t="shared" si="36"/>
         <v>0.50958356109947456</v>
       </c>
-      <c r="I87">
-        <f t="shared" si="35"/>
+      <c r="I87" s="11">
+        <f t="shared" si="36"/>
         <v>0.26849343489944899</v>
       </c>
-      <c r="J87">
-        <f t="shared" si="35"/>
+      <c r="J87" s="11">
+        <f t="shared" si="36"/>
         <v>-0.21413869147987413</v>
       </c>
-      <c r="K87">
-        <f t="shared" si="35"/>
+      <c r="K87" s="11">
+        <f t="shared" si="36"/>
         <v>-0.83061801685629855</v>
       </c>
-      <c r="L87">
-        <f t="shared" si="35"/>
+      <c r="L87" s="11">
+        <f t="shared" si="36"/>
         <v>-1.1065666703449759</v>
       </c>
-      <c r="M87">
-        <f t="shared" si="35"/>
+      <c r="M87" s="11">
+        <f t="shared" si="36"/>
         <v>-0.51257862041374957</v>
       </c>
-      <c r="N87">
-        <f t="shared" si="35"/>
+      <c r="N87" s="11">
+        <f t="shared" si="36"/>
         <v>0.29814239699997092</v>
       </c>
-      <c r="O87">
-        <f t="shared" si="35"/>
+      <c r="O87" s="11">
+        <f t="shared" si="36"/>
         <v>0.50436335008755007</v>
       </c>
-      <c r="P87">
-        <f t="shared" si="35"/>
+      <c r="P87" s="11">
+        <f t="shared" si="36"/>
         <v>0.21801833108109622</v>
       </c>
-      <c r="Q87">
-        <f t="shared" si="35"/>
+      <c r="Q87" s="11">
+        <f t="shared" si="36"/>
         <v>0.70249367527126816</v>
       </c>
-      <c r="R87">
-        <f t="shared" si="35"/>
+      <c r="R87" s="11">
+        <f t="shared" si="36"/>
         <v>-0.48905224320999935</v>
       </c>
-      <c r="S87">
-        <f t="shared" si="35"/>
+      <c r="S87" s="11">
+        <f t="shared" si="36"/>
         <v>0.25192505375512014</v>
       </c>
-      <c r="T87">
-        <f t="shared" si="35"/>
+      <c r="T87" s="11">
+        <f t="shared" si="36"/>
         <v>0.66248558643571465</v>
       </c>
-      <c r="U87">
-        <f t="shared" si="35"/>
+      <c r="U87" s="11">
+        <f t="shared" si="36"/>
         <v>-0.47309233328243294</v>
       </c>
-      <c r="V87">
-        <f t="shared" si="35"/>
+      <c r="V87" s="11">
+        <f t="shared" si="36"/>
         <v>-0.30637039002566313</v>
       </c>
-      <c r="W87">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="X87">
-        <f t="shared" si="35"/>
+      <c r="W87" s="11">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="X87" s="11">
+        <f t="shared" si="36"/>
         <v>-0.21366815983794593</v>
       </c>
     </row>
@@ -22373,5 +23363,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Analiza + wyniki - pt2
</commit_message>
<xml_diff>
--- a/wyniki.xlsx
+++ b/wyniki.xlsx
@@ -4046,6 +4046,549 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Średnia różnica ocen 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Wykresy!$B$14:$J$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.3846153846153846</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89743589743589736</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4615384615384617</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7692307692307692</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2307692307692313</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0769230769230775</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.92307692307692335</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.6923076923077538E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.30769230769230749</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Średnia róznica ocen 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Wykresy!$B$15:$J$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.3076923076923077</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1025641025641029</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6153846153846152</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4615384615384617</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0769230769230766</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61538461538461586</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15384615384615374</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.15384615384615419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.23076923076923084</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Średnia różnica wszystkich ocen</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Wykresy!$B$16:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.93589743589743568</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93589743589743568</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93589743589743568</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93589743589743568</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.93589743589743568</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.93589743589743568</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.93589743589743568</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.93589743589743568</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.93589743589743568</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="348794288"/>
+        <c:axId val="348793728"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="348794288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Numer pary</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> sekwencji</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t> filmowej</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="348793728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="348793728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Różnica ocen filmu</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="348794288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln cap="sq">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4167,6 +4710,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6218,6 +6801,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6339,6 +7425,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Wykres 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -13716,10 +14834,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y17"/>
+  <dimension ref="A1:Y19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14612,6 +15730,120 @@
         <v>1</v>
       </c>
     </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B14" s="11">
+        <f>ABS(B2-C2)</f>
+        <v>1.3846153846153846</v>
+      </c>
+      <c r="C14" s="11">
+        <f>ABS(D2-AVERAGE(E2:G2))</f>
+        <v>0.89743589743589736</v>
+      </c>
+      <c r="D14" s="11">
+        <f>ABS(H2-I2)</f>
+        <v>1.4615384615384617</v>
+      </c>
+      <c r="E14" s="11">
+        <f>ABS(J2-K2)</f>
+        <v>1.7692307692307692</v>
+      </c>
+      <c r="F14" s="11">
+        <f>ABS(L2-M2)</f>
+        <v>1.2307692307692313</v>
+      </c>
+      <c r="G14" s="11">
+        <f>ABS(N2-O2)</f>
+        <v>1.0769230769230775</v>
+      </c>
+      <c r="H14" s="11">
+        <f>ABS(P2-Q2)</f>
+        <v>0.92307692307692335</v>
+      </c>
+      <c r="I14" s="11">
+        <f>ABS(T2-U2)</f>
+        <v>7.6923076923077538E-2</v>
+      </c>
+      <c r="J14" s="11">
+        <f>ABS(W2-X2)</f>
+        <v>0.30769230769230749</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B15" s="11">
+        <f>ABS(B6-C6)</f>
+        <v>1.3076923076923077</v>
+      </c>
+      <c r="C15" s="11">
+        <f>ABS(D6-AVERAGE(E6:G6))</f>
+        <v>1.1025641025641029</v>
+      </c>
+      <c r="D15" s="11">
+        <f>ABS(H6-I6)</f>
+        <v>1.6153846153846152</v>
+      </c>
+      <c r="E15" s="11">
+        <f>ABS(J6-K6)</f>
+        <v>1.4615384615384617</v>
+      </c>
+      <c r="F15" s="11">
+        <f>ABS(L6-M6)</f>
+        <v>1.0769230769230766</v>
+      </c>
+      <c r="G15" s="11">
+        <f>ABS(N6-O6)</f>
+        <v>0.61538461538461586</v>
+      </c>
+      <c r="H15" s="11">
+        <f>ABS(P6-Q6)</f>
+        <v>0.15384615384615374</v>
+      </c>
+      <c r="I15" s="11">
+        <f>ABS(T6-U6)</f>
+        <v>0.15384615384615419</v>
+      </c>
+      <c r="J15" s="11">
+        <f>ABS(W6-X6)</f>
+        <v>0.23076923076923084</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B16" s="11">
+        <f>AVERAGE($B14:$J15)</f>
+        <v>0.93589743589743568</v>
+      </c>
+      <c r="C16" s="11">
+        <f>AVERAGE($B14:$J15)</f>
+        <v>0.93589743589743568</v>
+      </c>
+      <c r="D16" s="11">
+        <f t="shared" ref="C16:J16" si="0">AVERAGE($B14:$J15)</f>
+        <v>0.93589743589743568</v>
+      </c>
+      <c r="E16" s="11">
+        <f t="shared" si="0"/>
+        <v>0.93589743589743568</v>
+      </c>
+      <c r="F16" s="11">
+        <f t="shared" si="0"/>
+        <v>0.93589743589743568</v>
+      </c>
+      <c r="G16" s="11">
+        <f t="shared" si="0"/>
+        <v>0.93589743589743568</v>
+      </c>
+      <c r="H16" s="11">
+        <f t="shared" si="0"/>
+        <v>0.93589743589743568</v>
+      </c>
+      <c r="I16" s="11">
+        <f t="shared" si="0"/>
+        <v>0.93589743589743568</v>
+      </c>
+      <c r="J16" s="11">
+        <f t="shared" si="0"/>
+        <v>0.93589743589743568</v>
+      </c>
+    </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>113</v>
@@ -14681,6 +15913,12 @@
       </c>
       <c r="Y17" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f>LOG10(B2)</f>
+        <v>9.017663034908803E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wyniki - na wszelki wypadek
</commit_message>
<xml_diff>
--- a/wyniki.xlsx
+++ b/wyniki.xlsx
@@ -1989,11 +1989,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="173219616"/>
-        <c:axId val="173220176"/>
+        <c:axId val="164975616"/>
+        <c:axId val="164976176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="173219616"/>
+        <c:axId val="164975616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2091,7 +2091,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="173220176"/>
+        <c:crossAx val="164976176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2099,7 +2099,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="173220176"/>
+        <c:axId val="164976176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2206,7 +2206,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="173219616"/>
+        <c:crossAx val="164975616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2636,11 +2636,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="302021056"/>
-        <c:axId val="409505344"/>
+        <c:axId val="164698464"/>
+        <c:axId val="164699024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="302021056"/>
+        <c:axId val="164698464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2738,7 +2738,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="409505344"/>
+        <c:crossAx val="164699024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2746,7 +2746,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="409505344"/>
+        <c:axId val="164699024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2853,7 +2853,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302021056"/>
+        <c:crossAx val="164698464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3166,11 +3166,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="221191072"/>
-        <c:axId val="221191632"/>
+        <c:axId val="164702384"/>
+        <c:axId val="164702944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="221191072"/>
+        <c:axId val="164702384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3268,7 +3268,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221191632"/>
+        <c:crossAx val="164702944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3276,7 +3276,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="221191632"/>
+        <c:axId val="164702944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3383,7 +3383,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221191072"/>
+        <c:crossAx val="164702384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3741,11 +3741,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="315963760"/>
-        <c:axId val="309419584"/>
+        <c:axId val="165458368"/>
+        <c:axId val="165458928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="315963760"/>
+        <c:axId val="165458368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3777,7 +3777,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3843,7 +3842,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="309419584"/>
+        <c:crossAx val="165458928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3851,7 +3850,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="309419584"/>
+        <c:axId val="165458928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3897,7 +3896,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3958,7 +3956,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="315963760"/>
+        <c:crossAx val="165458368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4276,11 +4274,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="348794288"/>
-        <c:axId val="348793728"/>
+        <c:axId val="165462848"/>
+        <c:axId val="165463408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="348794288"/>
+        <c:axId val="165462848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4386,7 +4384,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348793728"/>
+        <c:crossAx val="165463408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4394,7 +4392,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348793728"/>
+        <c:axId val="165463408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4501,7 +4499,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348794288"/>
+        <c:crossAx val="165462848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14836,8 +14834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15816,7 +15814,7 @@
         <v>0.93589743589743568</v>
       </c>
       <c r="D16" s="11">
-        <f t="shared" ref="C16:J16" si="0">AVERAGE($B14:$J15)</f>
+        <f t="shared" ref="D16:J16" si="0">AVERAGE($B14:$J15)</f>
         <v>0.93589743589743568</v>
       </c>
       <c r="E16" s="11">

</xml_diff>

<commit_message>
wrzucam weź popraw formę żeby to ładnie wygladało
</commit_message>
<xml_diff>
--- a/wyniki.xlsx
+++ b/wyniki.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -1394,8 +1394,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1575,7 +1576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1614,8 +1615,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -5551,7 +5553,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5690,7 +5691,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5808,7 +5808,7 @@
             <c:numRef>
               <c:f>'Podzial po filmach'!$B$3:$J$3</c:f>
               <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1.2307692307692308</c:v>
@@ -5866,7 +5866,7 @@
             <c:numRef>
               <c:f>'Podzial po filmach'!$B$7:$J$7</c:f>
               <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1.0769230769230769</c:v>
@@ -5924,7 +5924,7 @@
             <c:numRef>
               <c:f>'Podzial po filmach'!$B$31:$J$31</c:f>
               <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2.6153846153846154</c:v>
@@ -5982,7 +5982,7 @@
             <c:numRef>
               <c:f>'Podzial po filmach'!$B$35:$J$35</c:f>
               <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2.3846153846153846</c:v>
@@ -6222,7 +6222,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6395,7 +6395,7 @@
             <c:numRef>
               <c:f>'Podzial po filmach'!$B$3:$J$3</c:f>
               <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1.2307692307692308</c:v>
@@ -6468,7 +6468,7 @@
             <c:numRef>
               <c:f>'Podzial po filmach'!$B$7:$J$7</c:f>
               <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1.0769230769230769</c:v>
@@ -6541,7 +6541,7 @@
             <c:numRef>
               <c:f>'Podzial po filmach'!$B$18:$J$18</c:f>
               <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2.6153846153846154</c:v>
@@ -6614,7 +6614,7 @@
             <c:numRef>
               <c:f>'Podzial po filmach'!$B$22:$J$22</c:f>
               <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2.3846153846153846</c:v>
@@ -19520,7 +19520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY19"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AS15" sqref="AS15"/>
     </sheetView>
   </sheetViews>
@@ -20421,7 +20421,7 @@
         <v>0.15384615384615397</v>
       </c>
       <c r="AD13">
-        <f t="shared" ref="AD13:BI13" si="0">C2-C6</f>
+        <f t="shared" ref="AD13:AY13" si="0">C2-C6</f>
         <v>0.23076923076923084</v>
       </c>
       <c r="AE13">
@@ -20894,8 +20894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N38" sqref="N37:N38"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20949,39 +20949,39 @@
       <c r="A3" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="24">
         <f>AVERAGE(WynikiScenariusza1!C1:C13)</f>
         <v>1.2307692307692308</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="24">
         <f>AVERAGE(WynikiScenariusza1!H1:H13)</f>
         <v>1.6153846153846154</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="24">
         <f>AVERAGE(WynikiScenariusza1!T1:T13)</f>
         <v>1.7692307692307692</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="24">
         <f>AVERAGE(WynikiScenariusza1!U1:U13)</f>
         <v>2.1538461538461537</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="24">
         <f>AVERAGE(WynikiScenariusza1!J1:J13)</f>
         <v>2.9230769230769229</v>
       </c>
-      <c r="G3" s="22">
+      <c r="G3" s="24">
         <f>AVERAGE(WynikiScenariusza1!K1:K13)</f>
         <v>3.3076923076923075</v>
       </c>
-      <c r="H3" s="22">
+      <c r="H3" s="24">
         <f>AVERAGE(WynikiScenariusza1!L1:L13)</f>
         <v>3.4615384615384617</v>
       </c>
-      <c r="I3" s="22">
+      <c r="I3" s="24">
         <f>AVERAGE(WynikiScenariusza1!I1:I13)</f>
         <v>4.1538461538461542</v>
       </c>
-      <c r="J3" s="22">
+      <c r="J3" s="24">
         <f>AVERAGE(WynikiScenariusza1!N1:N13)</f>
         <v>4.5384615384615383</v>
       </c>
@@ -21086,39 +21086,39 @@
       <c r="A7" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="24">
         <f>AVERAGE(WynikiScenariusza2!C1:C13)</f>
         <v>1.0769230769230769</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="24">
         <f>AVERAGE(WynikiScenariusza2!H1:H13)</f>
         <v>1.4615384615384615</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="24">
         <f>AVERAGE(WynikiScenariusza2!T1:T13)</f>
         <v>1.5384615384615385</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="24">
         <f>AVERAGE(WynikiScenariusza2!U1:U13)</f>
         <v>2.3076923076923075</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="24">
         <f>AVERAGE(WynikiScenariusza2!J1:J13)</f>
         <v>3</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="24">
         <f>AVERAGE(WynikiScenariusza2!K1:K13)</f>
         <v>3.5384615384615383</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="24">
         <f>AVERAGE(WynikiScenariusza2!L1:L13)</f>
         <v>3.8461538461538463</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="24">
         <f>AVERAGE(WynikiScenariusza2!I1:I13)</f>
         <v>4.0769230769230766</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="24">
         <f>AVERAGE(WynikiScenariusza2!N1:N13)</f>
         <v>4.4615384615384617</v>
       </c>
@@ -21241,31 +21241,31 @@
       <c r="A18" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="24">
         <v>2.6153846153846154</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="24">
         <v>2.5128205128205128</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="24">
         <v>3.2307692307692308</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="24">
         <v>3.9230769230769229</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="24">
         <v>4.1538461538461542</v>
       </c>
-      <c r="G18" s="22">
+      <c r="G18" s="24">
         <v>4.384615384615385</v>
       </c>
-      <c r="H18" s="22">
+      <c r="H18" s="24">
         <v>4.384615384615385</v>
       </c>
-      <c r="I18" s="22">
+      <c r="I18" s="24">
         <v>4.0769230769230766</v>
       </c>
-      <c r="J18" s="22">
+      <c r="J18" s="24">
         <v>4.8461538461538458</v>
       </c>
     </row>
@@ -21336,31 +21336,31 @@
       <c r="A22" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="24">
         <v>2.3846153846153846</v>
       </c>
-      <c r="C22" s="22">
+      <c r="C22" s="24">
         <v>2.5641025641025643</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="24">
         <v>3.1538461538461537</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="24">
         <v>3.7692307692307692</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="24">
         <v>4.0769230769230766</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="24">
         <v>4.1538461538461542</v>
       </c>
-      <c r="H22" s="22">
-        <v>4</v>
-      </c>
-      <c r="I22" s="22">
+      <c r="H22" s="24">
+        <v>4</v>
+      </c>
+      <c r="I22" s="24">
         <v>4.2307692307692308</v>
       </c>
-      <c r="J22" s="22">
+      <c r="J22" s="24">
         <v>4.6923076923076925</v>
       </c>
     </row>
@@ -21458,39 +21458,39 @@
       <c r="A31" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="22">
+      <c r="B31" s="24">
         <f>AVERAGE(WynikiScenariusza1!E1:E13)</f>
         <v>2.6153846153846154</v>
       </c>
-      <c r="C31" s="22">
+      <c r="C31" s="24">
         <f>AVERAGE(C45:E45)</f>
         <v>2.5128205128205128</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31" s="24">
         <f>AVERAGE(WynikiScenariusza1!S1:S13)</f>
         <v>3.2307692307692308</v>
       </c>
-      <c r="E31" s="22">
+      <c r="E31" s="24">
         <f>AVERAGE(WynikiScenariusza1!O1:O13)</f>
         <v>3.9230769230769229</v>
       </c>
-      <c r="F31" s="22">
+      <c r="F31" s="24">
         <f>AVERAGE(WynikiScenariusza1!P1:P13)</f>
         <v>4.1538461538461542</v>
       </c>
-      <c r="G31" s="22">
+      <c r="G31" s="24">
         <f>AVERAGE(WynikiScenariusza1!Q1:Q13)</f>
         <v>4.384615384615385</v>
       </c>
-      <c r="H31" s="22">
+      <c r="H31" s="24">
         <f>AVERAGE(WynikiScenariusza1!F1:F13)</f>
         <v>4.384615384615385</v>
       </c>
-      <c r="I31" s="22">
+      <c r="I31" s="24">
         <f>AVERAGE(WynikiScenariusza1!R1:R13)</f>
         <v>4.0769230769230766</v>
       </c>
-      <c r="J31" s="22">
+      <c r="J31" s="24">
         <f>AVERAGE(WynikiScenariusza1!D1:D13)</f>
         <v>4.8461538461538458</v>
       </c>
@@ -21589,39 +21589,39 @@
       <c r="A35" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="22">
+      <c r="B35" s="24">
         <f>AVERAGE(WynikiScenariusza2!E1:E13)</f>
         <v>2.3846153846153846</v>
       </c>
-      <c r="C35" s="22">
+      <c r="C35" s="24">
         <f>AVERAGE(C49:E49)</f>
         <v>2.5641025641025643</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D35" s="24">
         <f>AVERAGE(WynikiScenariusza2!S1:S13)</f>
         <v>3.1538461538461537</v>
       </c>
-      <c r="E35" s="22">
+      <c r="E35" s="24">
         <f>AVERAGE(WynikiScenariusza2!O1:O13)</f>
         <v>3.7692307692307692</v>
       </c>
-      <c r="F35" s="22">
+      <c r="F35" s="24">
         <f>AVERAGE(WynikiScenariusza2!P1:P13)</f>
         <v>4.0769230769230766</v>
       </c>
-      <c r="G35" s="22">
+      <c r="G35" s="24">
         <f>AVERAGE(WynikiScenariusza2!Q1:Q13)</f>
         <v>4.1538461538461542</v>
       </c>
-      <c r="H35" s="22">
+      <c r="H35" s="24">
         <f>AVERAGE(WynikiScenariusza2!F1:F13)</f>
         <v>4</v>
       </c>
-      <c r="I35" s="22">
+      <c r="I35" s="24">
         <f>AVERAGE(WynikiScenariusza2!R1:R13)</f>
         <v>4.2307692307692308</v>
       </c>
-      <c r="J35" s="22">
+      <c r="J35" s="24">
         <f>AVERAGE(WynikiScenariusza2!D1:D13)</f>
         <v>4.6923076923076925</v>
       </c>

</xml_diff>